<commit_message>
Update monitoring RKA 2026 dari web
</commit_message>
<xml_diff>
--- a/data/monitoring-rka-2026.xlsx
+++ b/data/monitoring-rka-2026.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/047618f1b9410114/Desktop/p3ste-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="191" documentId="11_2A22CECA176412FEE87DD0355E5DCE3AB74173C3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF437407-A069-44B4-91B7-7CC9FE93071A}"/>
+  <xr:revisionPtr revIDLastSave="193" documentId="11_2A22CECA176412FEE87DD0355E5DCE3AB74173C3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D7FACAA-E091-4D6C-8217-AF8DCE889327}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -180,12 +180,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -200,9 +206,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,7 +518,7 @@
       <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -557,8 +564,8 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2">
-        <v>0</v>
+      <c r="D2" s="2">
+        <v>1000000000</v>
       </c>
       <c r="E2">
         <v>0</v>

</xml_diff>